<commit_message>
Purchase Order TestScript 11to 15
</commit_message>
<xml_diff>
--- a/src/test/resources/vtiger_TC_Data.xlsx
+++ b/src/test/resources/vtiger_TC_Data.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15615" windowHeight="3600" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15555" windowHeight="3240" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CreateContactWithOrganizationIT" sheetId="1" r:id="rId1"/>
     <sheet name="CreateOrgonizationWithDifflist" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Creating New Purchase Order" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:P10"/>
+  <oleSize ref="A1:O11"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>TC_Parameter</t>
   </si>
@@ -77,19 +77,138 @@
   </si>
   <si>
     <t>Orgon info expected Result</t>
+  </si>
+  <si>
+    <r>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF545454"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Subject</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF545454"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> Billing Address</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF545454"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> Shipping Address</t>
+    </r>
+  </si>
+  <si>
+    <t>RowMaterial</t>
+  </si>
+  <si>
+    <t>Wardha</t>
+  </si>
+  <si>
+    <t>Banglore</t>
+  </si>
+  <si>
+    <r>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Item Name</t>
+    </r>
+  </si>
+  <si>
+    <t>List Price</t>
+  </si>
+  <si>
+    <t>Dress</t>
+  </si>
+  <si>
+    <t>2100</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Line item cannot be empty</t>
+  </si>
+  <si>
+    <t>Qty cannot be empty</t>
+  </si>
+  <si>
+    <t>Expected Result without qty</t>
+  </si>
+  <si>
+    <t>Expected Result without price and without item</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF545454"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -112,7 +231,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
@@ -121,6 +240,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -542,12 +665,93 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="29.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Listner Implemented in FrameWork
</commit_message>
<xml_diff>
--- a/src/test/resources/vtiger_TC_Data.xlsx
+++ b/src/test/resources/vtiger_TC_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15555" windowHeight="3240" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="16485" windowHeight="3240" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CreateContactWithOrganizationIT" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Creating New Purchase Order" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:O11"/>
+  <oleSize ref="A1:N9"/>
 </workbook>
 </file>
 
@@ -592,7 +592,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -667,7 +667,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>

</xml_diff>